<commit_message>
Update main script and tests
</commit_message>
<xml_diff>
--- a/circumpolar-race-results.xlsx
+++ b/circumpolar-race-results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Team Member</t>
   </si>
@@ -56,6 +56,36 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Sketch Ditty</t>
+  </si>
+  <si>
+    <t>David Eckardt</t>
+  </si>
+  <si>
+    <t>Phil Essam</t>
+  </si>
+  <si>
+    <t>Joshua Fosberg</t>
+  </si>
+  <si>
+    <t>Salley Hernandez</t>
+  </si>
+  <si>
+    <t>James Huller</t>
+  </si>
+  <si>
+    <t>Connie Karras</t>
+  </si>
+  <si>
+    <t>Zack Lever</t>
+  </si>
+  <si>
+    <t>David Ralston</t>
+  </si>
+  <si>
+    <t>Don Willis</t>
   </si>
 </sst>
 </file>
@@ -413,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -463,6 +493,446 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>305.89</v>
+      </c>
+      <c r="D2">
+        <v>236.83</v>
+      </c>
+      <c r="E2">
+        <v>200.29</v>
+      </c>
+      <c r="F2">
+        <v>199.29</v>
+      </c>
+      <c r="G2">
+        <v>40.75</v>
+      </c>
+      <c r="H2">
+        <v>164.14</v>
+      </c>
+      <c r="I2">
+        <v>173.41</v>
+      </c>
+      <c r="J2">
+        <v>278.86</v>
+      </c>
+      <c r="K2">
+        <v>225.63</v>
+      </c>
+      <c r="L2">
+        <v>269.49</v>
+      </c>
+      <c r="M2">
+        <v>193.55</v>
+      </c>
+      <c r="N2">
+        <v>2288.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>381.96</v>
+      </c>
+      <c r="C3">
+        <v>290.61</v>
+      </c>
+      <c r="D3">
+        <v>261.24</v>
+      </c>
+      <c r="E3">
+        <v>204.64</v>
+      </c>
+      <c r="F3">
+        <v>220.57</v>
+      </c>
+      <c r="G3">
+        <v>256.74</v>
+      </c>
+      <c r="H3">
+        <v>236.28</v>
+      </c>
+      <c r="I3">
+        <v>150.04</v>
+      </c>
+      <c r="J3">
+        <v>250.24</v>
+      </c>
+      <c r="K3">
+        <v>324.82</v>
+      </c>
+      <c r="L3">
+        <v>422.12</v>
+      </c>
+      <c r="M3">
+        <v>303.13</v>
+      </c>
+      <c r="N3">
+        <v>3302.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>47.38</v>
+      </c>
+      <c r="H4">
+        <v>48.6</v>
+      </c>
+      <c r="I4">
+        <v>10.24</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>77.09</v>
+      </c>
+      <c r="N4">
+        <v>183.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>234.72</v>
+      </c>
+      <c r="E5">
+        <v>247.23</v>
+      </c>
+      <c r="F5">
+        <v>154.7</v>
+      </c>
+      <c r="G5">
+        <v>116.4</v>
+      </c>
+      <c r="H5">
+        <v>61.08</v>
+      </c>
+      <c r="I5">
+        <v>98.68000000000001</v>
+      </c>
+      <c r="J5">
+        <v>308.57</v>
+      </c>
+      <c r="K5">
+        <v>407.1</v>
+      </c>
+      <c r="L5">
+        <v>242.28</v>
+      </c>
+      <c r="M5">
+        <v>136.85</v>
+      </c>
+      <c r="N5">
+        <v>2007.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>380.77</v>
+      </c>
+      <c r="D6">
+        <v>427.57</v>
+      </c>
+      <c r="E6">
+        <v>487.7</v>
+      </c>
+      <c r="F6">
+        <v>287.01</v>
+      </c>
+      <c r="G6">
+        <v>287.52</v>
+      </c>
+      <c r="H6">
+        <v>278.68</v>
+      </c>
+      <c r="I6">
+        <v>218.62</v>
+      </c>
+      <c r="J6">
+        <v>275.59</v>
+      </c>
+      <c r="K6">
+        <v>350.61</v>
+      </c>
+      <c r="L6">
+        <v>359.25</v>
+      </c>
+      <c r="M6">
+        <v>303.7</v>
+      </c>
+      <c r="N6">
+        <v>3657.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>195.12</v>
+      </c>
+      <c r="E7">
+        <v>209.25</v>
+      </c>
+      <c r="F7">
+        <v>151.7</v>
+      </c>
+      <c r="G7">
+        <v>119.1</v>
+      </c>
+      <c r="H7">
+        <v>76.34999999999999</v>
+      </c>
+      <c r="I7">
+        <v>80.83</v>
+      </c>
+      <c r="J7">
+        <v>188.98</v>
+      </c>
+      <c r="K7">
+        <v>240.16</v>
+      </c>
+      <c r="L7">
+        <v>85.20999999999999</v>
+      </c>
+      <c r="M7">
+        <v>95.88</v>
+      </c>
+      <c r="N7">
+        <v>1442.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>442.71</v>
+      </c>
+      <c r="C8">
+        <v>418.51</v>
+      </c>
+      <c r="D8">
+        <v>513.05</v>
+      </c>
+      <c r="E8">
+        <v>611.71</v>
+      </c>
+      <c r="F8">
+        <v>470.31</v>
+      </c>
+      <c r="G8">
+        <v>408.6</v>
+      </c>
+      <c r="H8">
+        <v>436.63</v>
+      </c>
+      <c r="I8">
+        <v>272.41</v>
+      </c>
+      <c r="J8">
+        <v>186.51</v>
+      </c>
+      <c r="K8">
+        <v>248.56</v>
+      </c>
+      <c r="L8">
+        <v>290.56</v>
+      </c>
+      <c r="M8">
+        <v>14.06</v>
+      </c>
+      <c r="N8">
+        <v>4313.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>300.09</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>233.36</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>294.77</v>
+      </c>
+      <c r="M9">
+        <v>271.38</v>
+      </c>
+      <c r="N9">
+        <v>1099.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>348.87</v>
+      </c>
+      <c r="C10">
+        <v>284.77</v>
+      </c>
+      <c r="D10">
+        <v>290.85</v>
+      </c>
+      <c r="E10">
+        <v>227.06</v>
+      </c>
+      <c r="F10">
+        <v>172.07</v>
+      </c>
+      <c r="G10">
+        <v>227.29</v>
+      </c>
+      <c r="H10">
+        <v>188.13</v>
+      </c>
+      <c r="I10">
+        <v>195.3</v>
+      </c>
+      <c r="J10">
+        <v>256.89</v>
+      </c>
+      <c r="K10">
+        <v>293.94</v>
+      </c>
+      <c r="L10">
+        <v>376.09</v>
+      </c>
+      <c r="M10">
+        <v>301.25</v>
+      </c>
+      <c r="N10">
+        <v>3162.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>421.37</v>
+      </c>
+      <c r="D11">
+        <v>447.33</v>
+      </c>
+      <c r="E11">
+        <v>533.47</v>
+      </c>
+      <c r="F11">
+        <v>443.21</v>
+      </c>
+      <c r="G11">
+        <v>333.6</v>
+      </c>
+      <c r="H11">
+        <v>265.75</v>
+      </c>
+      <c r="I11">
+        <v>221.49</v>
+      </c>
+      <c r="J11">
+        <v>291.48</v>
+      </c>
+      <c r="K11">
+        <v>296.29</v>
+      </c>
+      <c r="L11">
+        <v>345.23</v>
+      </c>
+      <c r="M11">
+        <v>150.38</v>
+      </c>
+      <c r="N11">
+        <v>3749.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>